<commit_message>
Initial analysis for CNPRM complete
</commit_message>
<xml_diff>
--- a/02_data/pda.xlsx
+++ b/02_data/pda.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F6FE8A-910B-45B6-8806-7CE8DEAE3590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93929695-D287-49FC-A48B-3BF3B500F7F3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6405" windowHeight="4365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6405" windowHeight="4365" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="or" sheetId="3" r:id="rId1"/>
     <sheet name="sucras" sheetId="4" r:id="rId2"/>
     <sheet name="rankings" sheetId="2" r:id="rId3"/>
+    <sheet name="rankings_td" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="31">
   <si>
     <t>closure</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>treatment</t>
+  </si>
+  <si>
+    <t>rpt_rx</t>
+  </si>
+  <si>
+    <t>sx</t>
   </si>
 </sst>
 </file>
@@ -462,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFE0242-4ADF-45F8-8B11-AEE9B1853761}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2297,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,7 +2320,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -2321,7 +2328,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -2345,7 +2352,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2365,6 +2372,93 @@
       </c>
       <c r="B9">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CBC0A9-2367-4E5A-92DF-5B8448FFE8B1}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>